<commit_message>
Update AsDpPractitionerProfile.fsh (#243) a100c0ecc15ff7b213c0d6a5165c6373eca26273
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-as-cs-intern-id-systems.xlsx
+++ b/main/ig/CodeSystem-as-cs-intern-id-systems.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0-snapshot-4</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T21:35:06+00:00</t>
+    <t>2024-11-14T08:22:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>